<commit_message>
Output regenerated after bug fixes were made in DiagnosticReport (My Health Record Pathology Report) profile.
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
@@ -1017,7 +1017,7 @@
 </t>
   </si>
   <si>
-    <t>Name/Code for this diagnostic report</t>
+    <t>Pathology test or test group</t>
   </si>
   <si>
     <t>A code or name that describes this diagnostic report.</t>
@@ -1144,7 +1144,7 @@
 Period</t>
   </si>
   <si>
-    <t>Clinically relevant time/time-period for report</t>
+    <t>Time of specimen collection</t>
   </si>
   <si>
     <t>The time or time-period the observed values are related to. When the subject of the report is a patient, this is usually either the time of the procedure or of specimen collection(s), but very often the source of the date/time is not known, only the date/time itself.</t>
@@ -1175,7 +1175,7 @@
 Date IssuedDate Verified</t>
   </si>
   <si>
-    <t>DateTime this version was made</t>
+    <t>Pathology report date time</t>
   </si>
   <si>
     <t>The date and time that this version of the report was made available to providers, typically after the report was reviewed and verified.</t>

</xml_diff>

<commit_message>
Completed DiagnosticReport (My Health Record Pathology Report) in Diagnostic Report FHIR IG
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3063" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3061" uniqueCount="563">
   <si>
     <t>Path</t>
   </si>
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-2:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-3:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-4:The requester of order details for pathology report that this diagnostic report is based on shall be a practitionerRole {basedOn.resolve().requester.resolve().where($this is PractitionerRole).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -213,81 +213,85 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-dir-1:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/diagnosticreport-path-mhr-1' {null}</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.meta.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.meta.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.meta.versionId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id
+</t>
+  </si>
+  <si>
+    <t>Version specific identifier</t>
+  </si>
+  <si>
+    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
+  </si>
+  <si>
+    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
+  </si>
+  <si>
+    <t>Meta.versionId</t>
+  </si>
+  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>DiagnosticReport.meta.id</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.meta.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.meta.versionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id
-</t>
-  </si>
-  <si>
-    <t>Version specific identifier</t>
-  </si>
-  <si>
-    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
-  </si>
-  <si>
-    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
-  </si>
-  <si>
-    <t>Meta.versionId</t>
-  </si>
-  <si>
     <t>DiagnosticReport.meta.lastUpdated</t>
   </si>
   <si>
@@ -956,7 +960,7 @@
     <t>Diagnostic services routinely issue provisional/incomplete reports, and sometimes withdraw previously released reports.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/diagnostic-report-status|4.0.1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/diagnosticreportstatus-report-available-1</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -998,7 +1002,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/diagnostic-service-sections</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/pathology-diagnostic-service-category-1</t>
   </si>
   <si>
     <t>OBR-24</t>
@@ -1023,10 +1027,7 @@
     <t>A code or name that describes this diagnostic report.</t>
   </si>
   <si>
-    <t>Codes that describe Diagnostic Reports.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/report-codes</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/pathology-procedure-1</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -1073,7 +1074,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -1203,7 +1204,7 @@
 ServicePractitionerDepartmentCompanyAuthorized byDirector</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/practitionerrole-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-ident-1)
 </t>
   </si>
   <si>
@@ -1955,7 +1956,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="64.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="82.98828125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -2738,7 +2739,7 @@
         <v>43</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>43</v>
@@ -2755,7 +2756,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -2778,16 +2779,16 @@
         <v>53</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2837,7 +2838,7 @@
         <v>43</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>41</v>
@@ -2849,7 +2850,7 @@
         <v>43</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ8" t="s" s="2">
         <v>43</v>
@@ -2866,7 +2867,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2889,16 +2890,16 @@
         <v>53</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2948,7 +2949,7 @@
         <v>43</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>41</v>
@@ -2960,7 +2961,7 @@
         <v>43</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>43</v>
@@ -2977,7 +2978,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -3000,16 +3001,16 @@
         <v>53</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -3059,7 +3060,7 @@
         <v>43</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>41</v>
@@ -3071,7 +3072,7 @@
         <v>43</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>43</v>
@@ -3088,7 +3089,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -3111,16 +3112,16 @@
         <v>53</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -3146,13 +3147,13 @@
         <v>43</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>43</v>
@@ -3170,7 +3171,7 @@
         <v>43</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>41</v>
@@ -3182,7 +3183,7 @@
         <v>43</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>43</v>
@@ -3199,7 +3200,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -3222,16 +3223,16 @@
         <v>53</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -3257,13 +3258,13 @@
         <v>43</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>43</v>
@@ -3281,7 +3282,7 @@
         <v>43</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>41</v>
@@ -3293,7 +3294,7 @@
         <v>43</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>43</v>
@@ -3310,7 +3311,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -3333,16 +3334,16 @@
         <v>53</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -3392,7 +3393,7 @@
         <v>43</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>41</v>
@@ -3404,7 +3405,7 @@
         <v>43</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>43</v>
@@ -3421,7 +3422,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3444,16 +3445,16 @@
         <v>43</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3461,7 +3462,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="R14" t="s" s="2">
         <v>43</v>
@@ -3479,13 +3480,13 @@
         <v>43</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>43</v>
@@ -3503,7 +3504,7 @@
         <v>43</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>41</v>
@@ -3515,7 +3516,7 @@
         <v>43</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>43</v>
@@ -3532,11 +3533,11 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -3555,16 +3556,16 @@
         <v>43</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3614,7 +3615,7 @@
         <v>43</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>41</v>
@@ -3626,7 +3627,7 @@
         <v>43</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>43</v>
@@ -3635,7 +3636,7 @@
         <v>43</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>43</v>
@@ -3643,11 +3644,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3666,16 +3667,16 @@
         <v>43</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -3725,7 +3726,7 @@
         <v>43</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>41</v>
@@ -3746,7 +3747,7 @@
         <v>43</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>43</v>
@@ -3754,7 +3755,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3783,7 +3784,7 @@
         <v>73</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M17" t="s" s="2">
         <v>75</v>
@@ -3836,7 +3837,7 @@
         <v>43</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -3857,7 +3858,7 @@
         <v>43</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>43</v>
@@ -3865,7 +3866,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3891,16 +3892,16 @@
         <v>72</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M18" t="s" s="2">
         <v>75</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>43</v>
@@ -3949,7 +3950,7 @@
         <v>43</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
@@ -3970,7 +3971,7 @@
         <v>43</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>43</v>
@@ -3978,11 +3979,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -4001,19 +4002,19 @@
         <v>53</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>43</v>
@@ -4050,7 +4051,7 @@
         <v>43</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AB19" s="2"/>
       <c r="AC19" t="s" s="2">
@@ -4060,7 +4061,7 @@
         <v>78</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>41</v>
@@ -4072,30 +4073,30 @@
         <v>43</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -4114,19 +4115,19 @@
         <v>53</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>43</v>
@@ -4175,7 +4176,7 @@
         <v>43</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -4187,24 +4188,24 @@
         <v>43</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -4313,7 +4314,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4424,7 +4425,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4447,19 +4448,19 @@
         <v>53</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>43</v>
@@ -4484,13 +4485,13 @@
         <v>43</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>43</v>
@@ -4508,7 +4509,7 @@
         <v>43</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
@@ -4520,16 +4521,16 @@
         <v>43</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>43</v>
@@ -4537,7 +4538,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4560,19 +4561,19 @@
         <v>53</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>43</v>
@@ -4597,11 +4598,11 @@
         <v>43</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>43</v>
@@ -4619,7 +4620,7 @@
         <v>43</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -4631,16 +4632,16 @@
         <v>43</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>43</v>
@@ -4648,7 +4649,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4757,7 +4758,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4868,7 +4869,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4891,19 +4892,19 @@
         <v>53</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>43</v>
@@ -4952,7 +4953,7 @@
         <v>43</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
@@ -4964,16 +4965,16 @@
         <v>43</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>43</v>
@@ -4981,7 +4982,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -5090,7 +5091,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5201,7 +5202,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5224,26 +5225,26 @@
         <v>53</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="R30" t="s" s="2">
         <v>43</v>
@@ -5285,7 +5286,7 @@
         <v>43</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -5297,16 +5298,16 @@
         <v>43</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>43</v>
@@ -5314,7 +5315,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5340,13 +5341,13 @@
         <v>54</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5396,7 +5397,7 @@
         <v>43</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -5408,16 +5409,16 @@
         <v>43</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>43</v>
@@ -5425,7 +5426,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5448,24 +5449,24 @@
         <v>53</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R32" t="s" s="2">
         <v>43</v>
@@ -5507,7 +5508,7 @@
         <v>43</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -5519,16 +5520,16 @@
         <v>43</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>43</v>
@@ -5536,7 +5537,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5562,14 +5563,14 @@
         <v>54</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>43</v>
@@ -5618,7 +5619,7 @@
         <v>43</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
@@ -5630,16 +5631,16 @@
         <v>43</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>43</v>
@@ -5647,7 +5648,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5670,19 +5671,19 @@
         <v>53</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>43</v>
@@ -5731,7 +5732,7 @@
         <v>43</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5743,16 +5744,16 @@
         <v>43</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>43</v>
@@ -5760,7 +5761,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5786,16 +5787,16 @@
         <v>54</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>43</v>
@@ -5844,7 +5845,7 @@
         <v>43</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>41</v>
@@ -5856,16 +5857,16 @@
         <v>43</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>43</v>
@@ -5873,7 +5874,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5896,19 +5897,19 @@
         <v>53</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>43</v>
@@ -5921,7 +5922,7 @@
         <v>43</v>
       </c>
       <c r="S36" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="T36" t="s" s="2">
         <v>43</v>
@@ -5957,7 +5958,7 @@
         <v>43</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5969,16 +5970,16 @@
         <v>43</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>43</v>
@@ -5986,7 +5987,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -6012,13 +6013,13 @@
         <v>54</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
@@ -6032,7 +6033,7 @@
         <v>43</v>
       </c>
       <c r="S37" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="T37" t="s" s="2">
         <v>43</v>
@@ -6068,7 +6069,7 @@
         <v>43</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -6080,16 +6081,16 @@
         <v>43</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>43</v>
@@ -6097,7 +6098,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6120,13 +6121,13 @@
         <v>53</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -6177,7 +6178,7 @@
         <v>43</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -6189,16 +6190,16 @@
         <v>43</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>43</v>
@@ -6206,7 +6207,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6229,16 +6230,16 @@
         <v>53</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -6288,7 +6289,7 @@
         <v>43</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -6300,16 +6301,16 @@
         <v>43</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>43</v>
@@ -6317,11 +6318,11 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -6340,19 +6341,19 @@
         <v>43</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>43</v>
@@ -6401,7 +6402,7 @@
         <v>43</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -6413,16 +6414,16 @@
         <v>43</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>43</v>
@@ -6430,7 +6431,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6453,17 +6454,17 @@
         <v>53</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>43</v>
@@ -6488,13 +6489,11 @@
         <v>43</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>301</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="X41" s="2"/>
       <c r="Y41" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>43</v>
@@ -6512,7 +6511,7 @@
         <v>43</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>52</v>
@@ -6524,32 +6523,32 @@
         <v>43</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F42" t="s" s="2">
         <v>42</v>
@@ -6564,16 +6563,16 @@
         <v>53</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6584,7 +6583,7 @@
         <v>43</v>
       </c>
       <c r="R42" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="S42" t="s" s="2">
         <v>43</v>
@@ -6599,11 +6598,11 @@
         <v>43</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="X42" s="2"/>
       <c r="Y42" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>43</v>
@@ -6621,7 +6620,7 @@
         <v>43</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -6633,28 +6632,28 @@
         <v>43</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6673,13 +6672,13 @@
         <v>53</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6706,11 +6705,9 @@
         <v>43</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="X43" t="s" s="2">
-        <v>323</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="X43" s="2"/>
       <c r="Y43" t="s" s="2">
         <v>324</v>
       </c>
@@ -6730,7 +6727,7 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>52</v>
@@ -6742,7 +6739,7 @@
         <v>43</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>325</v>
@@ -7002,19 +6999,19 @@
         <v>53</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O46" t="s" s="2">
         <v>43</v>
@@ -7061,7 +7058,7 @@
         <v>78</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -7073,16 +7070,16 @@
         <v>43</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>43</v>
@@ -7115,19 +7112,19 @@
         <v>53</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K47" t="s" s="2">
         <v>334</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>43</v>
@@ -7152,7 +7149,7 @@
         <v>43</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X47" s="2"/>
       <c r="Y47" t="s" s="2">
@@ -7174,7 +7171,7 @@
         <v>43</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -7186,16 +7183,16 @@
         <v>43</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>43</v>
@@ -7229,16 +7226,16 @@
         <v>54</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>43</v>
@@ -7287,7 +7284,7 @@
         <v>43</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -7299,16 +7296,16 @@
         <v>43</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>43</v>
@@ -7410,7 +7407,7 @@
         <v>43</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>343</v>
@@ -7523,7 +7520,7 @@
         <v>43</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>354</v>
@@ -7636,7 +7633,7 @@
         <v>43</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>365</v>
@@ -7676,7 +7673,7 @@
         <v>53</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K52" t="s" s="2">
         <v>371</v>
@@ -7749,7 +7746,7 @@
         <v>43</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>43</v>
@@ -7862,7 +7859,7 @@
         <v>43</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>385</v>
@@ -7975,7 +7972,7 @@
         <v>43</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>385</v>
@@ -8088,7 +8085,7 @@
         <v>43</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>43</v>
@@ -8201,7 +8198,7 @@
         <v>43</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>43</v>
@@ -8532,7 +8529,7 @@
         <v>419</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>43</v>
@@ -8541,7 +8538,7 @@
         <v>43</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>43</v>
@@ -8572,7 +8569,7 @@
         <v>53</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K60" t="s" s="2">
         <v>421</v>
@@ -8607,7 +8604,7 @@
         <v>43</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X60" t="s" s="2">
         <v>424</v>
@@ -8643,7 +8640,7 @@
         <v>43</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>43</v>
@@ -8652,7 +8649,7 @@
         <v>43</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>43</v>
@@ -8683,7 +8680,7 @@
         <v>53</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K61" t="s" s="2">
         <v>428</v>
@@ -8754,7 +8751,7 @@
         <v>43</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>43</v>
@@ -8865,7 +8862,7 @@
         <v>43</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>43</v>
@@ -8874,7 +8871,7 @@
         <v>43</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>43</v>
@@ -8976,7 +8973,7 @@
         <v>43</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>43</v>
@@ -9087,7 +9084,7 @@
         <v>43</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>43</v>
@@ -9359,7 +9356,7 @@
         <v>75</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>43</v>
@@ -9429,7 +9426,7 @@
         <v>43</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>43</v>
@@ -9533,7 +9530,7 @@
         <v>43</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>43</v>
@@ -9642,7 +9639,7 @@
         <v>43</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>43</v>
@@ -9753,7 +9750,7 @@
         <v>43</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ70" t="s" s="2">
         <v>43</v>
@@ -9793,7 +9790,7 @@
         <v>43</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K71" t="s" s="2">
         <v>477</v>
@@ -9826,7 +9823,7 @@
         <v>43</v>
       </c>
       <c r="W71" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="X71" t="s" s="2">
         <v>479</v>
@@ -9862,7 +9859,7 @@
         <v>43</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ71" t="s" s="2">
         <v>43</v>
@@ -10122,19 +10119,19 @@
         <v>53</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>43</v>
@@ -10181,7 +10178,7 @@
         <v>78</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -10193,16 +10190,16 @@
         <v>43</v>
       </c>
       <c r="AI74" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ74" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>43</v>
@@ -10235,19 +10232,19 @@
         <v>53</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K75" t="s" s="2">
         <v>487</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="N75" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="O75" t="s" s="2">
         <v>43</v>
@@ -10272,7 +10269,7 @@
         <v>43</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X75" t="s" s="2">
         <v>487</v>
@@ -10296,7 +10293,7 @@
         <v>43</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
@@ -10308,16 +10305,16 @@
         <v>43</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ75" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AM75" t="s" s="2">
         <v>43</v>
@@ -10351,16 +10348,16 @@
         <v>54</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N76" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>43</v>
@@ -10409,7 +10406,7 @@
         <v>43</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -10421,16 +10418,16 @@
         <v>43</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ76" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM76" t="s" s="2">
         <v>43</v>
@@ -10534,7 +10531,7 @@
         <v>43</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ77" t="s" s="2">
         <v>43</v>
@@ -10794,7 +10791,7 @@
         <v>53</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K80" t="s" s="2">
         <v>500</v>
@@ -10829,7 +10826,7 @@
         <v>43</v>
       </c>
       <c r="W80" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X80" t="s" s="2">
         <v>505</v>
@@ -10865,7 +10862,7 @@
         <v>43</v>
       </c>
       <c r="AI80" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ80" t="s" s="2">
         <v>43</v>
@@ -10905,7 +10902,7 @@
         <v>53</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K81" t="s" s="2">
         <v>511</v>
@@ -10928,7 +10925,7 @@
         <v>43</v>
       </c>
       <c r="S81" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T81" t="s" s="2">
         <v>43</v>
@@ -10940,13 +10937,13 @@
         <v>43</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="X81" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y81" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>43</v>
@@ -10976,7 +10973,7 @@
         <v>43</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ81" t="s" s="2">
         <v>43</v>
@@ -11089,7 +11086,7 @@
         <v>43</v>
       </c>
       <c r="AI82" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ82" t="s" s="2">
         <v>43</v>
@@ -11202,7 +11199,7 @@
         <v>43</v>
       </c>
       <c r="AI83" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ83" t="s" s="2">
         <v>43</v>
@@ -11315,7 +11312,7 @@
         <v>43</v>
       </c>
       <c r="AI84" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ84" t="s" s="2">
         <v>43</v>
@@ -11428,7 +11425,7 @@
         <v>43</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ85" t="s" s="2">
         <v>43</v>
@@ -11539,7 +11536,7 @@
         <v>43</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ86" t="s" s="2">
         <v>43</v>
@@ -11650,7 +11647,7 @@
         <v>43</v>
       </c>
       <c r="AI87" t="s" s="2">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AJ87" t="s" s="2">
         <v>43</v>

</xml_diff>

<commit_message>
MHR Pathology Diagnostic Report improvements
Added category known issue to DiagnosticReport and Observation profile.
Added implementation guidance to MHR Pathology Diagnostic Report
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-2:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-3:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-4:The requester of order details for pathology report that this diagnostic report is based on shall be a practitionerRole {basedOn.resolve().requester.resolve().where($this is PractitionerRole).exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-02:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-03:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-04:The requester of the pathology order shall be a PractitionerRole {basedOn.resolve().requester.resolve().where($this is PractitionerRole).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -214,7 +214,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-inv-dh-dir-1:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/diagnosticreport-path-mhr-1' {null}</t>
+inv-dh-dir-01:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/diagnosticreport-path-mhr-1' {null}</t>
   </si>
   <si>
     <t>DiagnosticReport.meta.id</t>
@@ -951,7 +951,7 @@
     <t>DiagnosticReport.status</t>
   </si>
   <si>
-    <t>registered | partial | preliminary | final +</t>
+    <t>partial | preliminary | final +</t>
   </si>
   <si>
     <t>The status of the diagnostic report.</t>

</xml_diff>

<commit_message>
Completed MHR Other DiagReport + MHR Imagin DiagReport in Diagnostics IG
Closes #47 and closes #44.
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-path-mhr-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$93</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3061" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3270" uniqueCount="569">
   <si>
     <t>Path</t>
   </si>
@@ -214,7 +214,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-inv-dh-dir-01:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/diagnosticreport-path-mhr-1' {null}</t>
+inv-dh-dir-01:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/diagnosticreport-path-mhr-1' {profile.where($this='http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/diagnosticreport-path-mhr-1').exists()}</t>
   </si>
   <si>
     <t>DiagnosticReport.meta.id</t>
@@ -927,7 +927,7 @@
 </t>
   </si>
   <si>
-    <t>What was requested</t>
+    <t>Pathology order</t>
   </si>
   <si>
     <t>Details concerning a service requested.</t>
@@ -946,6 +946,89 @@
   </si>
   <si>
     <t>outboundRelationship[typeCode=FLFS].target</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.basedOn.id</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.basedOn.extension</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.basedOn.reference</t>
+  </si>
+  <si>
+    <t>Literal reference, Relative, internal or absolute URL</t>
+  </si>
+  <si>
+    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
+  </si>
+  <si>
+    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
+  </si>
+  <si>
+    <t>Reference.reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref-1
+</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.basedOn.type</t>
+  </si>
+  <si>
+    <t>Type the reference refers to (e.g. "Patient")</t>
+  </si>
+  <si>
+    <t>The expected type of the target of the reference. If both Reference.type and Reference.reference are populated and Reference.reference is a FHIR URL, both SHALL be consistent.
+The type is the Canonical URL of Resource Definition that is the type this reference refers to. References are URLs that are relative to http://hl7.org/fhir/StructureDefinition/ e.g. "Patient" is a reference to http://hl7.org/fhir/StructureDefinition/Patient. Absolute URLs are only allowed for logical models (and can only be used in references in logical models, not resources).</t>
+  </si>
+  <si>
+    <t>This element is used to indicate the type of  the target of the reference. This may be used which ever of the other elements are populated (or not). In some cases, the type of the target may be determined by inspection of the reference (e.g. a RESTful URL) or by resolving the target of the reference; if both the type and a reference is provided, the reference SHALL resolve to a resource of the same type as that specified.</t>
+  </si>
+  <si>
+    <t>Aa resource (or, for logical models, the URI of the logical model).</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/resource-types</t>
+  </si>
+  <si>
+    <t>Reference.type</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.basedOn.identifier</t>
+  </si>
+  <si>
+    <t>Logical reference, when literal reference is not known</t>
+  </si>
+  <si>
+    <t>An identifier for the target resource. This is used when there is no way to reference the other resource directly, either because the entity it represents is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
+  </si>
+  <si>
+    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
+When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
+Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.
+Reference is intended to point to a structure that can potentially be expressed as a FHIR resource, though there is no need for it to exist as an actual FHIR resource instance - except in as much as an application wishes to actual find the target of the reference. The content referred to be the identifier must meet the logical constraints implied by any limitations on what resource types are permitted for the reference.  For example, it would not be legitimate to send the identifier for a drug prescription if the type were Reference(Observation|DiagnosticReport).  One of the use-cases for Reference.identifier is the situation where no FHIR representation exists (where the type is Reference (Any).</t>
+  </si>
+  <si>
+    <t>Reference.identifier</t>
+  </si>
+  <si>
+    <t>.identifier</t>
+  </si>
+  <si>
+    <t>DiagnosticReport.basedOn.display</t>
+  </si>
+  <si>
+    <t>Text alternative for the resource</t>
+  </si>
+  <si>
+    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
+  </si>
+  <si>
+    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
+  </si>
+  <si>
+    <t>Reference.display</t>
   </si>
   <si>
     <t>DiagnosticReport.status</t>
@@ -1315,78 +1398,13 @@
     <t>DiagnosticReport.result.reference</t>
   </si>
   <si>
-    <t>Literal reference, Relative, internal or absolute URL</t>
-  </si>
-  <si>
-    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
-  </si>
-  <si>
-    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
-  </si>
-  <si>
-    <t>Reference.reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref-1
-</t>
-  </si>
-  <si>
     <t>DiagnosticReport.result.type</t>
   </si>
   <si>
-    <t>Type the reference refers to (e.g. "Patient")</t>
-  </si>
-  <si>
-    <t>The expected type of the target of the reference. If both Reference.type and Reference.reference are populated and Reference.reference is a FHIR URL, both SHALL be consistent.
-The type is the Canonical URL of Resource Definition that is the type this reference refers to. References are URLs that are relative to http://hl7.org/fhir/StructureDefinition/ e.g. "Patient" is a reference to http://hl7.org/fhir/StructureDefinition/Patient. Absolute URLs are only allowed for logical models (and can only be used in references in logical models, not resources).</t>
-  </si>
-  <si>
-    <t>This element is used to indicate the type of  the target of the reference. This may be used which ever of the other elements are populated (or not). In some cases, the type of the target may be determined by inspection of the reference (e.g. a RESTful URL) or by resolving the target of the reference; if both the type and a reference is provided, the reference SHALL resolve to a resource of the same type as that specified.</t>
-  </si>
-  <si>
-    <t>Aa resource (or, for logical models, the URI of the logical model).</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/resource-types</t>
-  </si>
-  <si>
-    <t>Reference.type</t>
-  </si>
-  <si>
     <t>DiagnosticReport.result.identifier</t>
   </si>
   <si>
-    <t>Logical reference, when literal reference is not known</t>
-  </si>
-  <si>
-    <t>An identifier for the target resource. This is used when there is no way to reference the other resource directly, either because the entity it represents is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
-  </si>
-  <si>
-    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
-When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
-Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.
-Reference is intended to point to a structure that can potentially be expressed as a FHIR resource, though there is no need for it to exist as an actual FHIR resource instance - except in as much as an application wishes to actual find the target of the reference. The content referred to be the identifier must meet the logical constraints implied by any limitations on what resource types are permitted for the reference.  For example, it would not be legitimate to send the identifier for a drug prescription if the type were Reference(Observation|DiagnosticReport).  One of the use-cases for Reference.identifier is the situation where no FHIR representation exists (where the type is Reference (Any).</t>
-  </si>
-  <si>
-    <t>Reference.identifier</t>
-  </si>
-  <si>
-    <t>.identifier</t>
-  </si>
-  <si>
     <t>DiagnosticReport.result.display</t>
-  </si>
-  <si>
-    <t>Text alternative for the resource</t>
-  </si>
-  <si>
-    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
-  </si>
-  <si>
-    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
-  </si>
-  <si>
-    <t>Reference.display</t>
   </si>
   <si>
     <t>DiagnosticReport.imagingStudy</t>
@@ -1923,7 +1941,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM87"/>
+  <dimension ref="A1:AM93"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -6429,7 +6447,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
         <v>300</v>
       </c>
@@ -6439,33 +6457,31 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H41" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>301</v>
+        <v>66</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>302</v>
+        <v>67</v>
       </c>
       <c r="M41" s="2"/>
-      <c r="N41" t="s" s="2">
-        <v>303</v>
-      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>43</v>
       </c>
@@ -6489,11 +6505,13 @@
         <v>43</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="X41" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="Y41" t="s" s="2">
-        <v>304</v>
+        <v>43</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>43</v>
@@ -6511,10 +6529,10 @@
         <v>43</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>300</v>
+        <v>68</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>52</v>
@@ -6523,56 +6541,56 @@
         <v>43</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>305</v>
+        <v>43</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>306</v>
+        <v>43</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>307</v>
+        <v>69</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>308</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>310</v>
+        <v>71</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
-        <v>311</v>
+        <v>41</v>
       </c>
       <c r="F42" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>190</v>
+        <v>72</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>312</v>
+        <v>73</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>313</v>
+        <v>74</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>314</v>
+        <v>75</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6583,7 +6601,7 @@
         <v>43</v>
       </c>
       <c r="R42" t="s" s="2">
-        <v>315</v>
+        <v>43</v>
       </c>
       <c r="S42" t="s" s="2">
         <v>43</v>
@@ -6598,29 +6616,31 @@
         <v>43</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="X42" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="Y42" t="s" s="2">
-        <v>316</v>
+        <v>43</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AA42" t="s" s="2">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="AB42" t="s" s="2">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="AC42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD42" t="s" s="2">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>309</v>
+        <v>79</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -6632,28 +6652,28 @@
         <v>43</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>317</v>
+        <v>43</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>318</v>
+        <v>69</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>319</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>321</v>
+        <v>43</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6663,7 +6683,7 @@
         <v>52</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>43</v>
@@ -6672,15 +6692,17 @@
         <v>53</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>190</v>
+        <v>54</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="M43" s="2"/>
+        <v>304</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>305</v>
+      </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>43</v>
@@ -6705,11 +6727,13 @@
         <v>43</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="X43" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="Y43" t="s" s="2">
-        <v>324</v>
+        <v>43</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>43</v>
@@ -6727,36 +6751,36 @@
         <v>43</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>52</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>43</v>
+        <v>307</v>
       </c>
       <c r="AI43" t="s" s="2">
         <v>87</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>325</v>
+        <v>43</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>326</v>
+        <v>43</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>327</v>
+        <v>153</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>328</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6776,18 +6800,20 @@
         <v>43</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>66</v>
+        <v>309</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M44" s="2"/>
+        <v>310</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>311</v>
+      </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>43</v>
@@ -6812,13 +6838,13 @@
         <v>43</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>43</v>
+        <v>312</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>43</v>
+        <v>313</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>43</v>
@@ -6836,7 +6862,7 @@
         <v>43</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>68</v>
+        <v>314</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6848,7 +6874,7 @@
         <v>43</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>43</v>
@@ -6857,7 +6883,7 @@
         <v>43</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>43</v>
@@ -6865,18 +6891,18 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>43</v>
@@ -6885,19 +6911,19 @@
         <v>43</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>72</v>
+        <v>164</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>73</v>
+        <v>316</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>74</v>
+        <v>317</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>75</v>
+        <v>318</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6935,31 +6961,31 @@
         <v>43</v>
       </c>
       <c r="AA45" t="s" s="2">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="AB45" t="s" s="2">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="AC45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD45" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>79</v>
+        <v>319</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>43</v>
@@ -6968,7 +6994,7 @@
         <v>43</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>69</v>
+        <v>320</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>43</v>
@@ -6976,7 +7002,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6987,7 +7013,7 @@
         <v>41</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>43</v>
@@ -6999,20 +7025,18 @@
         <v>53</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>201</v>
+        <v>322</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>202</v>
+        <v>323</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>204</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>43</v>
       </c>
@@ -7048,23 +7072,25 @@
         <v>43</v>
       </c>
       <c r="AA46" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="AB46" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="AC46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD46" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>205</v>
+        <v>325</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>43</v>
@@ -7076,55 +7102,51 @@
         <v>43</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>206</v>
+        <v>43</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>207</v>
+        <v>153</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="47" hidden="true">
+    <row r="47">
       <c r="A47" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>333</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>53</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>204</v>
+        <v>329</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>43</v>
@@ -7153,7 +7175,7 @@
       </c>
       <c r="X47" s="2"/>
       <c r="Y47" t="s" s="2">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>43</v>
@@ -7171,13 +7193,13 @@
         <v>43</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>205</v>
+        <v>326</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>43</v>
@@ -7186,35 +7208,35 @@
         <v>87</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>43</v>
+        <v>331</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>206</v>
+        <v>332</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>207</v>
+        <v>333</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>43</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="48" hidden="true">
+    <row r="48">
       <c r="A48" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>43</v>
+        <v>336</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>41</v>
+        <v>337</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>43</v>
@@ -7223,20 +7245,18 @@
         <v>53</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>54</v>
+        <v>190</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>251</v>
+        <v>338</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>252</v>
+        <v>339</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>254</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>43</v>
       </c>
@@ -7245,7 +7265,7 @@
         <v>43</v>
       </c>
       <c r="R48" t="s" s="2">
-        <v>43</v>
+        <v>341</v>
       </c>
       <c r="S48" t="s" s="2">
         <v>43</v>
@@ -7260,13 +7280,11 @@
         <v>43</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X48" t="s" s="2">
-        <v>43</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="X48" s="2"/>
       <c r="Y48" t="s" s="2">
-        <v>43</v>
+        <v>342</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>43</v>
@@ -7284,13 +7302,13 @@
         <v>43</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>255</v>
+        <v>335</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>43</v>
@@ -7302,22 +7320,22 @@
         <v>43</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>256</v>
+        <v>343</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>257</v>
+        <v>344</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>43</v>
+        <v>345</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7336,18 +7354,16 @@
         <v>53</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>339</v>
+        <v>190</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="M49" s="2"/>
-      <c r="N49" t="s" s="2">
-        <v>342</v>
-      </c>
+      <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>43</v>
       </c>
@@ -7371,13 +7387,11 @@
         <v>43</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X49" t="s" s="2">
-        <v>43</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="X49" s="2"/>
       <c r="Y49" t="s" s="2">
-        <v>43</v>
+        <v>350</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>43</v>
@@ -7395,10 +7409,10 @@
         <v>43</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>52</v>
@@ -7410,25 +7424,25 @@
         <v>87</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>346</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>348</v>
+        <v>43</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7444,23 +7458,19 @@
         <v>43</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>349</v>
+        <v>54</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>350</v>
+        <v>66</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>353</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>43</v>
       </c>
@@ -7508,7 +7518,7 @@
         <v>43</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>347</v>
+        <v>68</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7520,60 +7530,58 @@
         <v>43</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>354</v>
+        <v>43</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>355</v>
+        <v>43</v>
       </c>
       <c r="AL50" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="AM50" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" hidden="true">
+      <c r="A51" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>359</v>
+        <v>71</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>360</v>
+        <v>72</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>361</v>
+        <v>73</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>362</v>
+        <v>74</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>364</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>43</v>
       </c>
@@ -7609,62 +7617,62 @@
         <v>43</v>
       </c>
       <c r="AA51" t="s" s="2">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD51" t="s" s="2">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>358</v>
+        <v>79</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>365</v>
+        <v>43</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>366</v>
+        <v>43</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>367</v>
+        <v>69</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>368</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>370</v>
+        <v>43</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>43</v>
@@ -7673,19 +7681,19 @@
         <v>53</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>371</v>
+        <v>201</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>372</v>
+        <v>202</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>373</v>
+        <v>203</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>374</v>
+        <v>204</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>43</v>
@@ -7722,25 +7730,23 @@
         <v>43</v>
       </c>
       <c r="AA52" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>43</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="AB52" s="2"/>
       <c r="AC52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD52" t="s" s="2">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>369</v>
+        <v>205</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>43</v>
@@ -7752,32 +7758,34 @@
         <v>43</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>375</v>
+        <v>206</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>376</v>
+        <v>207</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>377</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="B53" s="2"/>
+        <v>357</v>
+      </c>
+      <c r="B53" t="s" s="2">
+        <v>359</v>
+      </c>
       <c r="C53" t="s" s="2">
-        <v>379</v>
+        <v>43</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>43</v>
@@ -7786,19 +7794,19 @@
         <v>53</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>380</v>
+        <v>107</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>382</v>
+        <v>202</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>383</v>
+        <v>203</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>384</v>
+        <v>204</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>43</v>
@@ -7823,13 +7831,11 @@
         <v>43</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X53" t="s" s="2">
-        <v>43</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="X53" s="2"/>
       <c r="Y53" t="s" s="2">
-        <v>43</v>
+        <v>361</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>43</v>
@@ -7847,7 +7853,7 @@
         <v>43</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>378</v>
+        <v>205</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7862,32 +7868,32 @@
         <v>87</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>385</v>
+        <v>43</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>386</v>
+        <v>206</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>387</v>
+        <v>207</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>388</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>389</v>
+        <v>362</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>390</v>
+        <v>43</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>43</v>
@@ -7899,19 +7905,19 @@
         <v>53</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>391</v>
+        <v>54</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>392</v>
+        <v>251</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>393</v>
+        <v>252</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>394</v>
+        <v>253</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>384</v>
+        <v>254</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>43</v>
@@ -7960,13 +7966,13 @@
         <v>43</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>389</v>
+        <v>255</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>43</v>
@@ -7975,56 +7981,54 @@
         <v>87</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>385</v>
+        <v>43</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>395</v>
+        <v>256</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>387</v>
+        <v>257</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>388</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="55" hidden="true">
+    <row r="55">
       <c r="A55" t="s" s="2">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>43</v>
+        <v>364</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>397</v>
+        <v>365</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>398</v>
+        <v>366</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>400</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>401</v>
+        <v>368</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>43</v>
@@ -8073,13 +8077,13 @@
         <v>43</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>396</v>
+        <v>363</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG55" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH55" t="s" s="2">
         <v>43</v>
@@ -8088,56 +8092,56 @@
         <v>87</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>43</v>
+        <v>369</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>402</v>
+        <v>370</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>345</v>
+        <v>371</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>43</v>
+        <v>372</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>403</v>
+        <v>373</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>404</v>
+        <v>374</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I56" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="H56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I56" t="s" s="2">
-        <v>43</v>
-      </c>
       <c r="J56" t="s" s="2">
-        <v>405</v>
+        <v>375</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>406</v>
+        <v>376</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>409</v>
+        <v>379</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>43</v>
@@ -8186,13 +8190,13 @@
         <v>43</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>403</v>
+        <v>373</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>43</v>
@@ -8201,53 +8205,57 @@
         <v>87</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>43</v>
+        <v>380</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>410</v>
+        <v>381</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>411</v>
+        <v>382</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>43</v>
+        <v>383</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
-        <v>412</v>
+        <v>384</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>43</v>
+        <v>385</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F57" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>54</v>
+        <v>386</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>66</v>
+        <v>387</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
+        <v>388</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>390</v>
+      </c>
       <c r="O57" t="s" s="2">
         <v>43</v>
       </c>
@@ -8295,7 +8303,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>68</v>
+        <v>384</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -8307,58 +8315,60 @@
         <v>43</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>43</v>
+        <v>391</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>43</v>
+        <v>392</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>69</v>
+        <v>393</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>43</v>
+        <v>394</v>
       </c>
     </row>
-    <row r="58" hidden="true">
+    <row r="58">
       <c r="A58" t="s" s="2">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>71</v>
+        <v>396</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>73</v>
+        <v>397</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>74</v>
+        <v>398</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="N58" s="2"/>
+        <v>399</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>400</v>
+      </c>
       <c r="O58" t="s" s="2">
         <v>43</v>
       </c>
@@ -8394,62 +8404,62 @@
         <v>43</v>
       </c>
       <c r="AA58" t="s" s="2">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="AB58" t="s" s="2">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="AC58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD58" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>79</v>
+        <v>395</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>43</v>
+        <v>401</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>69</v>
+        <v>402</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>43</v>
+        <v>403</v>
       </c>
     </row>
-    <row r="59" hidden="true">
+    <row r="59">
       <c r="A59" t="s" s="2">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>43</v>
+        <v>405</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
         <v>52</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>43</v>
@@ -8458,18 +8468,20 @@
         <v>53</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>54</v>
+        <v>406</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="N59" s="2"/>
+        <v>409</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>410</v>
+      </c>
       <c r="O59" t="s" s="2">
         <v>43</v>
       </c>
@@ -8517,47 +8529,47 @@
         <v>43</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>419</v>
+        <v>43</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>87</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>43</v>
+        <v>411</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>43</v>
+        <v>412</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>153</v>
+        <v>413</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>43</v>
+        <v>414</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>43</v>
+        <v>416</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>43</v>
@@ -8569,18 +8581,20 @@
         <v>53</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>95</v>
+        <v>417</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="N60" s="2"/>
+        <v>420</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>410</v>
+      </c>
       <c r="O60" t="s" s="2">
         <v>43</v>
       </c>
@@ -8604,13 +8618,13 @@
         <v>43</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>424</v>
+        <v>43</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>425</v>
+        <v>43</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>43</v>
@@ -8628,13 +8642,13 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>43</v>
@@ -8643,21 +8657,21 @@
         <v>87</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>43</v>
+        <v>411</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>153</v>
+        <v>413</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>43</v>
+        <v>414</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8668,7 +8682,7 @@
         <v>41</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>43</v>
@@ -8677,21 +8691,23 @@
         <v>43</v>
       </c>
       <c r="I61" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>164</v>
+        <v>423</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="N61" s="2"/>
+        <v>426</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>427</v>
+      </c>
       <c r="O61" t="s" s="2">
         <v>43</v>
       </c>
@@ -8739,13 +8755,13 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>43</v>
@@ -8757,52 +8773,54 @@
         <v>43</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>43</v>
+        <v>428</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>432</v>
+        <v>371</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="62" hidden="true">
+    <row r="62">
       <c r="A62" t="s" s="2">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>43</v>
+        <v>430</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H62" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>54</v>
+        <v>431</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="M62" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="M62" t="s" s="2">
-        <v>436</v>
-      </c>
-      <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
         <v>43</v>
       </c>
@@ -8850,13 +8868,13 @@
         <v>43</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>43</v>
@@ -8868,10 +8886,10 @@
         <v>43</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>43</v>
+        <v>436</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>153</v>
+        <v>437</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>43</v>
@@ -8890,7 +8908,7 @@
         <v>41</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G63" t="s" s="2">
         <v>43</v>
@@ -8902,17 +8920,15 @@
         <v>43</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>439</v>
+        <v>54</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>440</v>
+        <v>66</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>441</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>442</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="M63" s="2"/>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>43</v>
@@ -8961,19 +8977,19 @@
         <v>43</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>438</v>
+        <v>68</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG63" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH63" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>43</v>
@@ -8982,7 +8998,7 @@
         <v>43</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>443</v>
+        <v>69</v>
       </c>
       <c r="AM63" t="s" s="2">
         <v>43</v>
@@ -8990,11 +9006,11 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>445</v>
+        <v>71</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
@@ -9010,21 +9026,21 @@
         <v>43</v>
       </c>
       <c r="I64" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>446</v>
+        <v>72</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>447</v>
+        <v>73</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="M64" s="2"/>
-      <c r="N64" t="s" s="2">
-        <v>449</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="M64" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>43</v>
       </c>
@@ -9060,19 +9076,19 @@
         <v>43</v>
       </c>
       <c r="AA64" t="s" s="2">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="AB64" t="s" s="2">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="AC64" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD64" t="s" s="2">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>444</v>
+        <v>79</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -9084,16 +9100,16 @@
         <v>43</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>450</v>
+        <v>43</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>411</v>
+        <v>69</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>43</v>
@@ -9101,7 +9117,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9109,7 +9125,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F65" t="s" s="2">
         <v>52</v>
@@ -9121,18 +9137,20 @@
         <v>43</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J65" t="s" s="2">
         <v>54</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>66</v>
+        <v>303</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M65" s="2"/>
+        <v>304</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>305</v>
+      </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>43</v>
@@ -9181,7 +9199,7 @@
         <v>43</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>68</v>
+        <v>306</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -9190,10 +9208,10 @@
         <v>52</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>43</v>
+        <v>307</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>43</v>
@@ -9202,7 +9220,7 @@
         <v>43</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>43</v>
@@ -9210,18 +9228,18 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>43</v>
@@ -9230,19 +9248,19 @@
         <v>43</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>73</v>
+        <v>309</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>74</v>
+        <v>310</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>75</v>
+        <v>311</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9268,13 +9286,13 @@
         <v>43</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>43</v>
+        <v>312</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>43</v>
+        <v>313</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>43</v>
@@ -9292,19 +9310,19 @@
         <v>43</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>79</v>
+        <v>314</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH66" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>43</v>
@@ -9313,7 +9331,7 @@
         <v>43</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>43</v>
@@ -9321,43 +9339,41 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>454</v>
+        <v>43</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="H67" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I67" t="s" s="2">
         <v>53</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>72</v>
+        <v>164</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>455</v>
+        <v>316</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>456</v>
+        <v>317</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>160</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>43</v>
       </c>
@@ -9405,19 +9421,19 @@
         <v>43</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>457</v>
+        <v>319</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>43</v>
@@ -9426,7 +9442,7 @@
         <v>43</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>153</v>
+        <v>320</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>43</v>
@@ -9434,7 +9450,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9454,23 +9470,21 @@
         <v>43</v>
       </c>
       <c r="I68" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J68" t="s" s="2">
         <v>54</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>459</v>
+        <v>322</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>460</v>
+        <v>323</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>461</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>462</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
         <v>43</v>
       </c>
@@ -9518,7 +9532,7 @@
         <v>43</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>458</v>
+        <v>325</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>41</v>
@@ -9539,7 +9553,7 @@
         <v>43</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>463</v>
+        <v>153</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>43</v>
@@ -9547,7 +9561,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9555,10 +9569,10 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G69" t="s" s="2">
         <v>43</v>
@@ -9567,18 +9581,20 @@
         <v>43</v>
       </c>
       <c r="I69" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>466</v>
+        <v>446</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>467</v>
-      </c>
-      <c r="M69" s="2"/>
+        <v>447</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>448</v>
+      </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
         <v>43</v>
@@ -9627,13 +9643,13 @@
         <v>43</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH69" t="s" s="2">
         <v>43</v>
@@ -9648,7 +9664,7 @@
         <v>43</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>468</v>
+        <v>449</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>43</v>
@@ -9656,18 +9672,18 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>470</v>
+        <v>451</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>43</v>
@@ -9676,20 +9692,20 @@
         <v>43</v>
       </c>
       <c r="I70" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>54</v>
+        <v>452</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" t="s" s="2">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>43</v>
@@ -9738,13 +9754,13 @@
         <v>43</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>469</v>
+        <v>450</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>43</v>
@@ -9756,10 +9772,10 @@
         <v>43</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>475</v>
+        <v>437</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>43</v>
@@ -9767,7 +9783,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9778,7 +9794,7 @@
         <v>41</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>43</v>
@@ -9790,13 +9806,13 @@
         <v>43</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>190</v>
+        <v>54</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>477</v>
+        <v>66</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>478</v>
+        <v>67</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -9823,13 +9839,13 @@
         <v>43</v>
       </c>
       <c r="W71" t="s" s="2">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="X71" t="s" s="2">
-        <v>479</v>
+        <v>43</v>
       </c>
       <c r="Y71" t="s" s="2">
-        <v>480</v>
+        <v>43</v>
       </c>
       <c r="Z71" t="s" s="2">
         <v>43</v>
@@ -9847,28 +9863,28 @@
         <v>43</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>476</v>
+        <v>68</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH71" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="AJ71" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>474</v>
+        <v>43</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>481</v>
+        <v>69</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>43</v>
@@ -9876,18 +9892,18 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F72" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G72" t="s" s="2">
         <v>43</v>
@@ -9899,15 +9915,17 @@
         <v>43</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M72" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>75</v>
+      </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>43</v>
@@ -9956,19 +9974,19 @@
         <v>43</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG72" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH72" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="AJ72" t="s" s="2">
         <v>43</v>
@@ -9985,11 +10003,11 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>71</v>
+        <v>460</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
@@ -10002,24 +10020,26 @@
         <v>43</v>
       </c>
       <c r="H73" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J73" t="s" s="2">
         <v>72</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>73</v>
+        <v>461</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>74</v>
+        <v>462</v>
       </c>
       <c r="M73" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="N73" s="2"/>
+      <c r="N73" t="s" s="2">
+        <v>160</v>
+      </c>
       <c r="O73" t="s" s="2">
         <v>43</v>
       </c>
@@ -10055,19 +10075,19 @@
         <v>43</v>
       </c>
       <c r="AA73" t="s" s="2">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="AB73" t="s" s="2">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="AC73" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD73" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>79</v>
+        <v>463</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
@@ -10088,7 +10108,7 @@
         <v>43</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>43</v>
@@ -10096,7 +10116,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>484</v>
+        <v>464</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10107,7 +10127,7 @@
         <v>41</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>43</v>
@@ -10116,22 +10136,22 @@
         <v>43</v>
       </c>
       <c r="I74" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>201</v>
+        <v>465</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>202</v>
+        <v>466</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>203</v>
+        <v>467</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>204</v>
+        <v>468</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>43</v>
@@ -10168,23 +10188,25 @@
         <v>43</v>
       </c>
       <c r="AA74" t="s" s="2">
-        <v>485</v>
-      </c>
-      <c r="AB74" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="AB74" t="s" s="2">
+        <v>43</v>
+      </c>
       <c r="AC74" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD74" t="s" s="2">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>205</v>
+        <v>464</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG74" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH74" t="s" s="2">
         <v>43</v>
@@ -10196,10 +10218,10 @@
         <v>43</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>206</v>
+        <v>43</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>207</v>
+        <v>469</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>43</v>
@@ -10207,17 +10229,15 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>486</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
         <v>43</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F75" t="s" s="2">
         <v>52</v>
@@ -10232,20 +10252,16 @@
         <v>53</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>107</v>
+        <v>471</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>204</v>
-      </c>
+        <v>473</v>
+      </c>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
         <v>43</v>
       </c>
@@ -10269,13 +10285,13 @@
         <v>43</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>184</v>
+        <v>43</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>487</v>
+        <v>43</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>488</v>
+        <v>43</v>
       </c>
       <c r="Z75" t="s" s="2">
         <v>43</v>
@@ -10293,13 +10309,13 @@
         <v>43</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>205</v>
+        <v>470</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>43</v>
@@ -10311,10 +10327,10 @@
         <v>43</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>206</v>
+        <v>43</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>207</v>
+        <v>474</v>
       </c>
       <c r="AM75" t="s" s="2">
         <v>43</v>
@@ -10322,11 +10338,11 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>43</v>
+        <v>476</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
@@ -10342,22 +10358,20 @@
         <v>43</v>
       </c>
       <c r="I76" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J76" t="s" s="2">
         <v>54</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>251</v>
+        <v>477</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>253</v>
-      </c>
+        <v>478</v>
+      </c>
+      <c r="M76" s="2"/>
       <c r="N76" t="s" s="2">
-        <v>254</v>
+        <v>479</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>43</v>
@@ -10406,7 +10420,7 @@
         <v>43</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>255</v>
+        <v>475</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -10424,18 +10438,18 @@
         <v>43</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>256</v>
+        <v>480</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>257</v>
+        <v>481</v>
       </c>
       <c r="AM76" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10443,13 +10457,13 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>43</v>
@@ -10458,20 +10472,16 @@
         <v>43</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>491</v>
+        <v>190</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>495</v>
-      </c>
+        <v>484</v>
+      </c>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
         <v>43</v>
       </c>
@@ -10495,13 +10505,13 @@
         <v>43</v>
       </c>
       <c r="W77" t="s" s="2">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>43</v>
+        <v>485</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>43</v>
+        <v>486</v>
       </c>
       <c r="Z77" t="s" s="2">
         <v>43</v>
@@ -10519,7 +10529,7 @@
         <v>43</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>41</v>
@@ -10537,10 +10547,10 @@
         <v>43</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>43</v>
@@ -10548,7 +10558,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10657,7 +10667,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10768,7 +10778,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10776,10 +10786,10 @@
       </c>
       <c r="D80" s="2"/>
       <c r="E80" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G80" t="s" s="2">
         <v>43</v>
@@ -10791,30 +10801,32 @@
         <v>53</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>500</v>
+        <v>201</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>501</v>
-      </c>
-      <c r="M80" s="2"/>
+        <v>202</v>
+      </c>
+      <c r="M80" t="s" s="2">
+        <v>203</v>
+      </c>
       <c r="N80" t="s" s="2">
-        <v>502</v>
+        <v>204</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P80" s="2"/>
       <c r="Q80" t="s" s="2">
-        <v>503</v>
+        <v>43</v>
       </c>
       <c r="R80" t="s" s="2">
         <v>43</v>
       </c>
       <c r="S80" t="s" s="2">
-        <v>504</v>
+        <v>43</v>
       </c>
       <c r="T80" t="s" s="2">
         <v>43</v>
@@ -10826,37 +10838,35 @@
         <v>43</v>
       </c>
       <c r="W80" t="s" s="2">
-        <v>184</v>
+        <v>43</v>
       </c>
       <c r="X80" t="s" s="2">
-        <v>505</v>
+        <v>43</v>
       </c>
       <c r="Y80" t="s" s="2">
-        <v>506</v>
+        <v>43</v>
       </c>
       <c r="Z80" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AA80" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB80" t="s" s="2">
-        <v>43</v>
-      </c>
+        <v>491</v>
+      </c>
+      <c r="AB80" s="2"/>
       <c r="AC80" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD80" t="s" s="2">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>507</v>
+        <v>205</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG80" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH80" t="s" s="2">
         <v>43</v>
@@ -10868,10 +10878,10 @@
         <v>43</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>508</v>
+        <v>206</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>509</v>
+        <v>207</v>
       </c>
       <c r="AM80" t="s" s="2">
         <v>43</v>
@@ -10879,9 +10889,11 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>510</v>
-      </c>
-      <c r="B81" s="2"/>
+        <v>490</v>
+      </c>
+      <c r="B81" t="s" s="2">
+        <v>492</v>
+      </c>
       <c r="C81" t="s" s="2">
         <v>43</v>
       </c>
@@ -10902,17 +10914,19 @@
         <v>53</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>512</v>
-      </c>
-      <c r="M81" s="2"/>
+        <v>202</v>
+      </c>
+      <c r="M81" t="s" s="2">
+        <v>203</v>
+      </c>
       <c r="N81" t="s" s="2">
-        <v>513</v>
+        <v>204</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>43</v>
@@ -10925,7 +10939,7 @@
         <v>43</v>
       </c>
       <c r="S81" t="s" s="2">
-        <v>133</v>
+        <v>43</v>
       </c>
       <c r="T81" t="s" s="2">
         <v>43</v>
@@ -10937,13 +10951,13 @@
         <v>43</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="X81" t="s" s="2">
-        <v>135</v>
+        <v>493</v>
       </c>
       <c r="Y81" t="s" s="2">
-        <v>136</v>
+        <v>494</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>43</v>
@@ -10961,13 +10975,13 @@
         <v>43</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>514</v>
+        <v>205</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG81" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH81" t="s" s="2">
         <v>43</v>
@@ -10979,10 +10993,10 @@
         <v>43</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>43</v>
+        <v>206</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>515</v>
+        <v>207</v>
       </c>
       <c r="AM81" t="s" s="2">
         <v>43</v>
@@ -10990,7 +11004,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -11010,22 +11024,22 @@
         <v>43</v>
       </c>
       <c r="I82" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>517</v>
+        <v>54</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>518</v>
+        <v>251</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>519</v>
+        <v>252</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>520</v>
+        <v>253</v>
       </c>
       <c r="N82" t="s" s="2">
-        <v>521</v>
+        <v>254</v>
       </c>
       <c r="O82" t="s" s="2">
         <v>43</v>
@@ -11074,7 +11088,7 @@
         <v>43</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>522</v>
+        <v>255</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -11092,18 +11106,18 @@
         <v>43</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>523</v>
+        <v>256</v>
       </c>
       <c r="AL82" t="s" s="2">
-        <v>524</v>
+        <v>257</v>
       </c>
       <c r="AM82" t="s" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="83" hidden="true">
+    <row r="83">
       <c r="A83" t="s" s="2">
-        <v>525</v>
+        <v>496</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -11117,28 +11131,28 @@
         <v>52</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="H83" t="s" s="2">
         <v>43</v>
       </c>
       <c r="I83" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>526</v>
+        <v>497</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>527</v>
+        <v>498</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>528</v>
+        <v>499</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>530</v>
+        <v>501</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>43</v>
@@ -11151,7 +11165,7 @@
         <v>43</v>
       </c>
       <c r="S83" t="s" s="2">
-        <v>531</v>
+        <v>43</v>
       </c>
       <c r="T83" t="s" s="2">
         <v>43</v>
@@ -11187,13 +11201,13 @@
         <v>43</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>43</v>
@@ -11205,10 +11219,10 @@
         <v>43</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>533</v>
+        <v>480</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>534</v>
+        <v>502</v>
       </c>
       <c r="AM83" t="s" s="2">
         <v>43</v>
@@ -11216,7 +11230,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>535</v>
+        <v>503</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -11236,23 +11250,19 @@
         <v>43</v>
       </c>
       <c r="I84" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>536</v>
+        <v>54</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>537</v>
+        <v>66</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>538</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>539</v>
-      </c>
-      <c r="N84" t="s" s="2">
-        <v>540</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
         <v>43</v>
       </c>
@@ -11300,7 +11310,7 @@
         <v>43</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>541</v>
+        <v>68</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
@@ -11312,7 +11322,7 @@
         <v>43</v>
       </c>
       <c r="AI84" t="s" s="2">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="AJ84" t="s" s="2">
         <v>43</v>
@@ -11321,7 +11331,7 @@
         <v>43</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>542</v>
+        <v>69</v>
       </c>
       <c r="AM84" t="s" s="2">
         <v>43</v>
@@ -11329,18 +11339,18 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>543</v>
+        <v>504</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>43</v>
@@ -11349,23 +11359,21 @@
         <v>43</v>
       </c>
       <c r="I85" t="s" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>517</v>
+        <v>72</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>544</v>
+        <v>73</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>545</v>
+        <v>74</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>546</v>
-      </c>
-      <c r="N85" t="s" s="2">
-        <v>547</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
         <v>43</v>
       </c>
@@ -11401,31 +11409,31 @@
         <v>43</v>
       </c>
       <c r="AA85" t="s" s="2">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="AB85" t="s" s="2">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="AC85" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AD85" t="s" s="2">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>548</v>
+        <v>79</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AH85" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AJ85" t="s" s="2">
         <v>43</v>
@@ -11434,7 +11442,7 @@
         <v>43</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>549</v>
+        <v>69</v>
       </c>
       <c r="AM85" t="s" s="2">
         <v>43</v>
@@ -11442,7 +11450,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>550</v>
+        <v>505</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11465,30 +11473,30 @@
         <v>53</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>551</v>
+        <v>506</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>552</v>
+        <v>507</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" t="s" s="2">
-        <v>553</v>
+        <v>508</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>43</v>
       </c>
       <c r="P86" s="2"/>
       <c r="Q86" t="s" s="2">
-        <v>43</v>
+        <v>509</v>
       </c>
       <c r="R86" t="s" s="2">
         <v>43</v>
       </c>
       <c r="S86" t="s" s="2">
-        <v>554</v>
+        <v>510</v>
       </c>
       <c r="T86" t="s" s="2">
         <v>43</v>
@@ -11500,13 +11508,13 @@
         <v>43</v>
       </c>
       <c r="W86" t="s" s="2">
-        <v>43</v>
+        <v>184</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>43</v>
+        <v>511</v>
       </c>
       <c r="Y86" t="s" s="2">
-        <v>43</v>
+        <v>512</v>
       </c>
       <c r="Z86" t="s" s="2">
         <v>43</v>
@@ -11524,7 +11532,7 @@
         <v>43</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>555</v>
+        <v>513</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
@@ -11542,10 +11550,10 @@
         <v>43</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>43</v>
+        <v>514</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>556</v>
+        <v>515</v>
       </c>
       <c r="AM86" t="s" s="2">
         <v>43</v>
@@ -11553,7 +11561,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>557</v>
+        <v>516</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11576,17 +11584,17 @@
         <v>53</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>558</v>
+        <v>129</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>559</v>
+        <v>517</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>560</v>
+        <v>518</v>
       </c>
       <c r="M87" s="2"/>
       <c r="N87" t="s" s="2">
-        <v>561</v>
+        <v>519</v>
       </c>
       <c r="O87" t="s" s="2">
         <v>43</v>
@@ -11599,7 +11607,7 @@
         <v>43</v>
       </c>
       <c r="S87" t="s" s="2">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="T87" t="s" s="2">
         <v>43</v>
@@ -11611,13 +11619,13 @@
         <v>43</v>
       </c>
       <c r="W87" t="s" s="2">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="X87" t="s" s="2">
-        <v>43</v>
+        <v>135</v>
       </c>
       <c r="Y87" t="s" s="2">
-        <v>43</v>
+        <v>136</v>
       </c>
       <c r="Z87" t="s" s="2">
         <v>43</v>
@@ -11635,7 +11643,7 @@
         <v>43</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>562</v>
+        <v>520</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>41</v>
@@ -11656,14 +11664,688 @@
         <v>43</v>
       </c>
       <c r="AL87" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="AM87" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" hidden="true">
+      <c r="A88" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F88" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J88" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="K88" t="s" s="2">
+        <v>524</v>
+      </c>
+      <c r="L88" t="s" s="2">
+        <v>525</v>
+      </c>
+      <c r="M88" t="s" s="2">
+        <v>526</v>
+      </c>
+      <c r="N88" t="s" s="2">
+        <v>527</v>
+      </c>
+      <c r="O88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P88" s="2"/>
+      <c r="Q88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK88" t="s" s="2">
+        <v>529</v>
+      </c>
+      <c r="AL88" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="AM88" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" hidden="true">
+      <c r="A89" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="F89" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I89" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J89" t="s" s="2">
+        <v>532</v>
+      </c>
+      <c r="K89" t="s" s="2">
+        <v>533</v>
+      </c>
+      <c r="L89" t="s" s="2">
+        <v>534</v>
+      </c>
+      <c r="M89" t="s" s="2">
+        <v>535</v>
+      </c>
+      <c r="N89" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="O89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P89" s="2"/>
+      <c r="Q89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S89" t="s" s="2">
+        <v>537</v>
+      </c>
+      <c r="T89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE89" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="AF89" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG89" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI89" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AJ89" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK89" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="AL89" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="AM89" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" hidden="true">
+      <c r="A90" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F90" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I90" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J90" t="s" s="2">
         <v>542</v>
       </c>
-      <c r="AM87" t="s" s="2">
+      <c r="K90" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="L90" t="s" s="2">
+        <v>544</v>
+      </c>
+      <c r="M90" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="N90" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="O90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P90" s="2"/>
+      <c r="Q90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE90" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="AF90" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG90" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI90" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AJ90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK90" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL90" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="AM90" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" hidden="true">
+      <c r="A91" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="F91" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I91" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J91" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="K91" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="L91" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="M91" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="N91" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="O91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P91" s="2"/>
+      <c r="Q91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE91" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL91" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AM91" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" hidden="true">
+      <c r="A92" t="s" s="2">
+        <v>556</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="F92" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>557</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="M92" s="2"/>
+      <c r="N92" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="O92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P92" s="2"/>
+      <c r="Q92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S92" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>561</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>562</v>
+      </c>
+      <c r="AM92" t="s" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" hidden="true">
+      <c r="A93" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F93" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>565</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>566</v>
+      </c>
+      <c r="M93" s="2"/>
+      <c r="N93" t="s" s="2">
+        <v>567</v>
+      </c>
+      <c r="O93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="P93" s="2"/>
+      <c r="Q93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>568</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="AM93" t="s" s="2">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM87">
+  <autoFilter ref="A1:AM93">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -11673,7 +12355,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI86">
+  <conditionalFormatting sqref="A2:AI92">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>